<commit_message>
More formatting of spreadsheet in dialog
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>date</t>
   </si>
@@ -195,19 +195,300 @@
   </si>
   <si>
     <t>Vince White</t>
+  </si>
+  <si>
+    <r>
+      <t>Minim</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>qui</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dolore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>eu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>pariatur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>eu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>cupidatat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>sint</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>esse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dolore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>elit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>labore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>proident</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF9CDCFE"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>officia</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>something</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,9 +511,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,12 +797,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP5"/>
+  <dimension ref="A1:AP6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6765" topLeftCell="AB1" activePane="topRight"/>
-      <selection activeCell="C5" sqref="C5"/>
-      <selection pane="topRight" activeCell="AH4" sqref="AH4"/>
+      <pane xSplit="6765" topLeftCell="AB1"/>
+      <selection activeCell="C6" sqref="C6"/>
+      <selection pane="topRight" activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -731,7 +1015,19 @@
         <v>45</v>
       </c>
     </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44086</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Switch to a data grid
This isn't a clear win. We get locking of the 1st column, but at  the price of much harder formatting.
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
   <si>
     <t>date</t>
   </si>
@@ -464,13 +464,19 @@
   </si>
   <si>
     <t>something</t>
+  </si>
+  <si>
+    <t>Conversation</t>
+  </si>
+  <si>
+    <t>Bogus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +493,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF9CDCFE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFCE9178"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -511,10 +523,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -797,28 +812,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AP6"/>
+  <dimension ref="A1:AQ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6765" topLeftCell="AB1"/>
+      <pane xSplit="6765" activePane="topRight"/>
       <selection activeCell="C6" sqref="C6"/>
-      <selection pane="topRight" activeCell="AE13" sqref="AE13"/>
+      <selection pane="topRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" customWidth="1"/>
-    <col min="32" max="32" width="17.7109375" customWidth="1"/>
-    <col min="33" max="33" width="30.140625" customWidth="1"/>
-    <col min="34" max="34" width="19.42578125" customWidth="1"/>
-    <col min="35" max="35" width="21.140625" customWidth="1"/>
-    <col min="39" max="39" width="18" customWidth="1"/>
-    <col min="41" max="41" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="33" max="33" width="17.7109375" customWidth="1"/>
+    <col min="34" max="34" width="30.140625" customWidth="1"/>
+    <col min="35" max="35" width="19.42578125" customWidth="1"/>
+    <col min="36" max="36" width="21.140625" customWidth="1"/>
+    <col min="40" max="40" width="18" customWidth="1"/>
+    <col min="42" max="42" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -829,124 +845,124 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44357</v>
       </c>
@@ -956,26 +972,29 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="AH2" t="s">
         <v>51</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>45</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>52</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>53</v>
       </c>
-      <c r="AM2" t="s">
+      <c r="AN2" t="s">
         <v>54</v>
       </c>
-      <c r="AO2" t="s">
+      <c r="AP2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
         <v>48</v>
@@ -984,38 +1003,41 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" t="s">
         <v>44</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44084</v>
       </c>
       <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>52</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44085</v>
       </c>
       <c r="C5" t="s">
         <v>50</v>
       </c>
-      <c r="AH5" t="s">
+      <c r="AI5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44086</v>
       </c>

</xml_diff>

<commit_message>
Import dlg now showing all mappings & row selections working
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
   <si>
     <t>date</t>
   </si>
@@ -470,6 +470,12 @@
   </si>
   <si>
     <t>Bogus</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Australasia</t>
   </si>
 </sst>
 </file>
@@ -817,7 +823,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6765" activePane="topRight"/>
       <selection activeCell="C6" sqref="C6"/>
-      <selection pane="topRight" activeCell="E6" sqref="E6"/>
+      <selection pane="topRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,6 +832,9 @@
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
+    <col min="9" max="9" width="18" customWidth="1"/>
     <col min="33" max="33" width="17.7109375" customWidth="1"/>
     <col min="34" max="34" width="30.140625" customWidth="1"/>
     <col min="35" max="35" width="19.42578125" customWidth="1"/>
@@ -975,6 +984,9 @@
       <c r="D2" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="G2" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="AH2" t="s">
         <v>51</v>
       </c>
@@ -1007,6 +1019,9 @@
       </c>
       <c r="E3" t="s">
         <v>44</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="AH3" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Import custom fields, mark newly imported sessions
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>date</t>
   </si>
@@ -476,6 +476,9 @@
   </si>
   <si>
     <t>Australasia</t>
+  </si>
+  <si>
+    <t>Zoom</t>
   </si>
 </sst>
 </file>
@@ -821,9 +824,9 @@
   <dimension ref="A1:AQ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6765" activePane="topRight"/>
+      <pane xSplit="6765" topLeftCell="M1" activePane="topRight"/>
       <selection activeCell="C6" sqref="C6"/>
-      <selection pane="topRight" activeCell="G3" sqref="G3"/>
+      <selection pane="topRight" activeCell="AD12" sqref="AD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,6 +990,9 @@
       <c r="G2" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="AD2" t="s">
+        <v>63</v>
+      </c>
       <c r="AH2" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
Force UTF8 import of spreadsheets
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>date</t>
   </si>
@@ -479,13 +479,16 @@
   </si>
   <si>
     <t>Zoom</t>
+  </si>
+  <si>
+    <t>สระ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,6 +514,12 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202122"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -532,7 +541,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -541,6 +550,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,8 +835,8 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="6765" topLeftCell="M1" activePane="topRight"/>
-      <selection activeCell="C6" sqref="C6"/>
-      <selection pane="topRight" activeCell="AD12" sqref="AD12"/>
+      <selection activeCell="B6" sqref="B6"/>
+      <selection pane="topRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,6 +1000,9 @@
       <c r="G2" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="N2" s="4" t="s">
+        <v>64</v>
+      </c>
       <c r="AD2" t="s">
         <v>63</v>
       </c>

</xml_diff>

<commit_message>
Tell what permitted values are if a value isn't allowed
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -475,13 +475,13 @@
     <t>Australia</t>
   </si>
   <si>
-    <t>Australasia</t>
-  </si>
-  <si>
     <t>Zoom</t>
   </si>
   <si>
     <t>สระ</t>
+  </si>
+  <si>
+    <t>Gondwana</t>
   </si>
 </sst>
 </file>
@@ -834,8 +834,8 @@
   <dimension ref="A1:AQ6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6765" topLeftCell="M1" activePane="topRight"/>
-      <selection activeCell="B6" sqref="B6"/>
+      <pane xSplit="18555" topLeftCell="M1"/>
+      <selection activeCell="G6" activeCellId="1" sqref="G3 G6"/>
       <selection pane="topRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -1001,10 +1001,10 @@
         <v>61</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AH2" t="s">
         <v>51</v>
@@ -1040,7 +1040,7 @@
         <v>44</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="AH3" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
More import problem tips
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -469,9 +469,6 @@
     <t>Conversation</t>
   </si>
   <si>
-    <t>Bogus</t>
-  </si>
-  <si>
     <t>Australia</t>
   </si>
   <si>
@@ -482,6 +479,9 @@
   </si>
   <si>
     <t>Gondwana</t>
+  </si>
+  <si>
+    <t>Rap</t>
   </si>
 </sst>
 </file>
@@ -835,7 +835,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="18555" topLeftCell="M1"/>
-      <selection activeCell="G6" activeCellId="1" sqref="G3 G6"/>
+      <selection activeCell="E5" sqref="E5"/>
       <selection pane="topRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -998,13 +998,13 @@
         <v>59</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AD2" t="s">
         <v>61</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>62</v>
       </c>
       <c r="AH2" t="s">
         <v>51</v>
@@ -1034,13 +1034,13 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AH3" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
Validate and Import archive-specific access choices
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
   <si>
     <t>date</t>
   </si>
@@ -482,13 +482,64 @@
   </si>
   <si>
     <t>Rap</t>
+  </si>
+  <si>
+    <t>RC</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>bogus</t>
+  </si>
+  <si>
+    <t>Time Limit</t>
+  </si>
+  <si>
+    <t>Level 1: Public access</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Protected</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>REAP users</t>
+  </si>
+  <si>
+    <t>EnTiTy</t>
+  </si>
+  <si>
+    <t>some reason</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>another explanation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,6 +571,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -541,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -551,6 +615,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,8 +901,8 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="18555" topLeftCell="M1"/>
-      <selection activeCell="E5" sqref="E5"/>
-      <selection pane="topRight" activeCell="O8" sqref="O8"/>
+      <selection activeCell="D10" sqref="D10"/>
+      <selection pane="topRight" activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,10 +910,18 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="16" max="16" width="27.42578125" customWidth="1"/>
+    <col min="17" max="17" width="21.140625" customWidth="1"/>
+    <col min="18" max="18" width="18" customWidth="1"/>
     <col min="33" max="33" width="17.7109375" customWidth="1"/>
     <col min="34" max="34" width="30.140625" customWidth="1"/>
     <col min="35" max="35" width="19.42578125" customWidth="1"/>
@@ -867,76 +941,76 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="S1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="U1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="W1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="X1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Y1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Z1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AA1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AB1" t="s">
         <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>26</v>
       </c>
       <c r="AC1" t="s">
         <v>27</v>
@@ -994,13 +1068,40 @@
       <c r="C2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="W2" s="4" t="s">
         <v>62</v>
       </c>
       <c r="AD2" t="s">
@@ -1034,12 +1135,27 @@
         <v>43</v>
       </c>
       <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" t="s">
         <v>64</v>
       </c>
-      <c r="E3" t="s">
+      <c r="N3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>63</v>
       </c>
       <c r="AH3" t="s">
@@ -1053,6 +1169,15 @@
       <c r="B4" t="s">
         <v>49</v>
       </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" t="s">
+        <v>80</v>
+      </c>
       <c r="AH4" t="s">
         <v>52</v>
       </c>
@@ -1066,6 +1191,9 @@
       </c>
       <c r="C5" t="s">
         <v>50</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
       </c>
       <c r="AI5" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Add validation for bad dates on import
</commit_message>
<xml_diff>
--- a/sample data/LingMetaX.xlsx
+++ b/sample data/LingMetaX.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="84">
   <si>
     <t>date</t>
   </si>
@@ -533,6 +533,12 @@
   </si>
   <si>
     <t>another explanation</t>
+  </si>
+  <si>
+    <t>Yesterday</t>
+  </si>
+  <si>
+    <t>bad date</t>
   </si>
 </sst>
 </file>
@@ -897,11 +903,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ6"/>
+  <dimension ref="A1:AQ7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="18555" topLeftCell="M1"/>
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B11" sqref="B11"/>
       <selection pane="topRight" activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
@@ -1210,6 +1216,17 @@
         <v>58</v>
       </c>
     </row>
+    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>